<commit_message>
Add valores a receber
</commit_message>
<xml_diff>
--- a/saida.xlsx
+++ b/saida.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -377,6 +377,11 @@
           <t>POSTO</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>VALOR</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -390,6 +395,9 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
+      <c r="D2" t="n">
+        <v>456</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -403,6 +411,9 @@
       <c r="C3" t="n">
         <v>1</v>
       </c>
+      <c r="D3" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -416,6 +427,9 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
+      <c r="D4" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -429,6 +443,9 @@
       <c r="C5" t="n">
         <v>1</v>
       </c>
+      <c r="D5" t="n">
+        <v>551</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -442,6 +459,9 @@
       <c r="C6" t="n">
         <v>1</v>
       </c>
+      <c r="D6" t="n">
+        <v>152</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -455,6 +475,9 @@
       <c r="C7" t="n">
         <v>1</v>
       </c>
+      <c r="D7" t="n">
+        <v>475</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -468,6 +491,9 @@
       <c r="C8" t="n">
         <v>1</v>
       </c>
+      <c r="D8" t="n">
+        <v>513</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -481,6 +507,9 @@
       <c r="C9" t="n">
         <v>1</v>
       </c>
+      <c r="D9" t="n">
+        <v>380</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -494,6 +523,9 @@
       <c r="C10" t="n">
         <v>1</v>
       </c>
+      <c r="D10" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -507,6 +539,9 @@
       <c r="C11" t="n">
         <v>1</v>
       </c>
+      <c r="D11" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -520,6 +555,9 @@
       <c r="C12" t="n">
         <v>1</v>
       </c>
+      <c r="D12" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -533,6 +571,9 @@
       <c r="C13" t="n">
         <v>1</v>
       </c>
+      <c r="D13" t="n">
+        <v>114</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -546,6 +587,9 @@
       <c r="C14" t="n">
         <v>1</v>
       </c>
+      <c r="D14" t="n">
+        <v>266</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -559,6 +603,9 @@
       <c r="C15" t="n">
         <v>1</v>
       </c>
+      <c r="D15" t="n">
+        <v>380</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -572,6 +619,9 @@
       <c r="C16" t="n">
         <v>1</v>
       </c>
+      <c r="D16" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -585,6 +635,9 @@
       <c r="C17" t="n">
         <v>1</v>
       </c>
+      <c r="D17" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -598,6 +651,9 @@
       <c r="C18" t="n">
         <v>1</v>
       </c>
+      <c r="D18" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -611,6 +667,9 @@
       <c r="C19" t="n">
         <v>1</v>
       </c>
+      <c r="D19" t="n">
+        <v>494</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -624,6 +683,9 @@
       <c r="C20" t="n">
         <v>1</v>
       </c>
+      <c r="D20" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -637,6 +699,9 @@
       <c r="C21" t="n">
         <v>1</v>
       </c>
+      <c r="D21" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -650,6 +715,9 @@
       <c r="C22" t="n">
         <v>1</v>
       </c>
+      <c r="D22" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
@@ -663,6 +731,9 @@
       <c r="C23" t="n">
         <v>1</v>
       </c>
+      <c r="D23" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
@@ -676,6 +747,9 @@
       <c r="C24" t="n">
         <v>2</v>
       </c>
+      <c r="D24" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -689,6 +763,9 @@
       <c r="C25" t="n">
         <v>2</v>
       </c>
+      <c r="D25" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -702,6 +779,9 @@
       <c r="C26" t="n">
         <v>2</v>
       </c>
+      <c r="D26" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -715,6 +795,9 @@
       <c r="C27" t="n">
         <v>2</v>
       </c>
+      <c r="D27" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -728,6 +811,9 @@
       <c r="C28" t="n">
         <v>2</v>
       </c>
+      <c r="D28" t="n">
+        <v>513</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
@@ -741,6 +827,9 @@
       <c r="C29" t="n">
         <v>2</v>
       </c>
+      <c r="D29" t="n">
+        <v>513</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
@@ -754,6 +843,9 @@
       <c r="C30" t="n">
         <v>2</v>
       </c>
+      <c r="D30" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
@@ -767,6 +859,9 @@
       <c r="C31" t="n">
         <v>2</v>
       </c>
+      <c r="D31" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
@@ -780,6 +875,9 @@
       <c r="C32" t="n">
         <v>2</v>
       </c>
+      <c r="D32" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
@@ -793,6 +891,9 @@
       <c r="C33" t="n">
         <v>2</v>
       </c>
+      <c r="D33" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -806,6 +907,9 @@
       <c r="C34" t="n">
         <v>3</v>
       </c>
+      <c r="D34" t="n">
+        <v>266</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
@@ -819,6 +923,9 @@
       <c r="C35" t="n">
         <v>3</v>
       </c>
+      <c r="D35" t="n">
+        <v>323</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
@@ -832,6 +939,9 @@
       <c r="C36" t="n">
         <v>3</v>
       </c>
+      <c r="D36" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
@@ -845,6 +955,9 @@
       <c r="C37" t="n">
         <v>3</v>
       </c>
+      <c r="D37" t="n">
+        <v>209</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
@@ -858,6 +971,9 @@
       <c r="C38" t="n">
         <v>3</v>
       </c>
+      <c r="D38" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
@@ -871,6 +987,9 @@
       <c r="C39" t="n">
         <v>3</v>
       </c>
+      <c r="D39" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -884,11 +1003,14 @@
       <c r="C40" t="n">
         <v>3</v>
       </c>
+      <c r="D40" t="n">
+        <v>380</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>FABRICIO DEMATTE !</t>
+          <t xml:space="preserve">FABRICIO DEMATTE </t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -897,6 +1019,9 @@
       <c r="C41" t="n">
         <v>3</v>
       </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
@@ -910,6 +1035,9 @@
       <c r="C42" t="n">
         <v>3</v>
       </c>
+      <c r="D42" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
@@ -923,6 +1051,9 @@
       <c r="C43" t="n">
         <v>3</v>
       </c>
+      <c r="D43" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
@@ -936,6 +1067,9 @@
       <c r="C44" t="n">
         <v>3</v>
       </c>
+      <c r="D44" t="n">
+        <v>323</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
@@ -949,6 +1083,9 @@
       <c r="C45" t="n">
         <v>3</v>
       </c>
+      <c r="D45" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
@@ -962,6 +1099,9 @@
       <c r="C46" t="n">
         <v>6</v>
       </c>
+      <c r="D46" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
@@ -975,6 +1115,9 @@
       <c r="C47" t="n">
         <v>6</v>
       </c>
+      <c r="D47" t="n">
+        <v>551</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
@@ -988,11 +1131,14 @@
       <c r="C48" t="n">
         <v>6</v>
       </c>
+      <c r="D48" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>CRISTIANO FREITAS BARBOZA !</t>
+          <t xml:space="preserve">CRISTIANO FREITAS BARBOZA </t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -1001,6 +1147,9 @@
       <c r="C49" t="n">
         <v>6</v>
       </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -1014,6 +1163,9 @@
       <c r="C50" t="n">
         <v>6</v>
       </c>
+      <c r="D50" t="n">
+        <v>114</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
@@ -1027,6 +1179,9 @@
       <c r="C51" t="n">
         <v>6</v>
       </c>
+      <c r="D51" t="n">
+        <v>551</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
@@ -1040,6 +1195,9 @@
       <c r="C52" t="n">
         <v>6</v>
       </c>
+      <c r="D52" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
@@ -1053,6 +1211,9 @@
       <c r="C53" t="n">
         <v>6</v>
       </c>
+      <c r="D53" t="n">
+        <v>513</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -1066,6 +1227,9 @@
       <c r="C54" t="n">
         <v>6</v>
       </c>
+      <c r="D54" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
@@ -1079,6 +1243,9 @@
       <c r="C55" t="n">
         <v>6</v>
       </c>
+      <c r="D55" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -1092,6 +1259,9 @@
       <c r="C56" t="n">
         <v>6</v>
       </c>
+      <c r="D56" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -1105,6 +1275,9 @@
       <c r="C57" t="n">
         <v>6</v>
       </c>
+      <c r="D57" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
@@ -1118,6 +1291,9 @@
       <c r="C58" t="n">
         <v>6</v>
       </c>
+      <c r="D58" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
@@ -1131,6 +1307,9 @@
       <c r="C59" t="n">
         <v>7</v>
       </c>
+      <c r="D59" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
@@ -1144,6 +1323,9 @@
       <c r="C60" t="n">
         <v>7</v>
       </c>
+      <c r="D60" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
@@ -1157,6 +1339,9 @@
       <c r="C61" t="n">
         <v>7</v>
       </c>
+      <c r="D61" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
@@ -1170,6 +1355,9 @@
       <c r="C62" t="n">
         <v>7</v>
       </c>
+      <c r="D62" t="n">
+        <v>513</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
@@ -1183,6 +1371,9 @@
       <c r="C63" t="n">
         <v>7</v>
       </c>
+      <c r="D63" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
@@ -1196,6 +1387,9 @@
       <c r="C64" t="n">
         <v>7</v>
       </c>
+      <c r="D64" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
@@ -1209,6 +1403,9 @@
       <c r="C65" t="n">
         <v>7</v>
       </c>
+      <c r="D65" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="inlineStr">
@@ -1222,6 +1419,9 @@
       <c r="C66" t="n">
         <v>7</v>
       </c>
+      <c r="D66" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
@@ -1235,6 +1435,9 @@
       <c r="C67" t="n">
         <v>7</v>
       </c>
+      <c r="D67" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="inlineStr">
@@ -1248,6 +1451,9 @@
       <c r="C68" t="n">
         <v>7</v>
       </c>
+      <c r="D68" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
@@ -1261,6 +1467,9 @@
       <c r="C69" t="n">
         <v>7</v>
       </c>
+      <c r="D69" t="n">
+        <v>380</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="inlineStr">
@@ -1274,6 +1483,9 @@
       <c r="C70" t="n">
         <v>7</v>
       </c>
+      <c r="D70" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="inlineStr">
@@ -1287,6 +1499,9 @@
       <c r="C71" t="n">
         <v>9</v>
       </c>
+      <c r="D71" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
@@ -1300,6 +1515,9 @@
       <c r="C72" t="n">
         <v>9</v>
       </c>
+      <c r="D72" t="n">
+        <v>532</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
@@ -1313,11 +1531,14 @@
       <c r="C73" t="n">
         <v>9</v>
       </c>
+      <c r="D73" t="n">
+        <v>551</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>MELQUISEDEC DE SOUSA !</t>
+          <t xml:space="preserve">MELQUISEDEC DE SOUSA </t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -1326,6 +1547,9 @@
       <c r="C74" t="n">
         <v>9</v>
       </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="inlineStr">
@@ -1339,6 +1563,9 @@
       <c r="C75" t="n">
         <v>9</v>
       </c>
+      <c r="D75" t="n">
+        <v>266</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="inlineStr">
@@ -1352,6 +1579,9 @@
       <c r="C76" t="n">
         <v>9</v>
       </c>
+      <c r="D76" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
@@ -1365,6 +1595,9 @@
       <c r="C77" t="n">
         <v>9</v>
       </c>
+      <c r="D77" t="n">
+        <v>513</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
@@ -1378,6 +1611,9 @@
       <c r="C78" t="n">
         <v>9</v>
       </c>
+      <c r="D78" t="n">
+        <v>532</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
@@ -1391,11 +1627,14 @@
       <c r="C79" t="n">
         <v>9</v>
       </c>
+      <c r="D79" t="n">
+        <v>532</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="inlineStr">
         <is>
-          <t>ANDRE LUIS CARLINI DA SILVA !</t>
+          <t xml:space="preserve">ANDRE LUIS CARLINI DA SILVA </t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1404,6 +1643,9 @@
       <c r="C80" t="n">
         <v>9</v>
       </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="inlineStr">
@@ -1417,6 +1659,9 @@
       <c r="C81" t="n">
         <v>9</v>
       </c>
+      <c r="D81" t="n">
+        <v>532</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
@@ -1430,17 +1675,23 @@
       <c r="C82" t="n">
         <v>9</v>
       </c>
+      <c r="D82" t="n">
+        <v>285</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>VICTOR HUGO BALDA CYPRIANO !</t>
+          <t xml:space="preserve">VICTOR HUGO BALDA CYPRIANO </t>
         </is>
       </c>
       <c r="B83" t="n">
         <v>0</v>
       </c>
       <c r="C83" t="inlineStr"/>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>